<commit_message>
them chuc nang random theo location
</commit_message>
<xml_diff>
--- a/Excel_info.xlsx
+++ b/Excel_info.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MyPC\OneDrive\Desktop\HSA_REGISTER\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MyPC\OneDrive\Desktop\HSA_REGISTER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDAD6DE4-8745-4092-AF91-18983AED65F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B59AEA5C-4D8D-4E06-8F1C-D4EAFD105D7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="1440" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34470" yWindow="8520" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Tài khoản</t>
   </si>
@@ -49,46 +49,25 @@
 1- Đăng kí random</t>
   </si>
   <si>
-    <t>123</t>
+    <t>tk2504200@gmail.com</t>
+  </si>
+  <si>
+    <t>Khanh2504</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>24124</t>
-  </si>
-  <si>
-    <t>1244</t>
-  </si>
-  <si>
-    <t>2341234</t>
-  </si>
-  <si>
-    <t>14134</t>
-  </si>
-  <si>
-    <t>134</t>
-  </si>
-  <si>
-    <t>414</t>
-  </si>
-  <si>
-    <t>341</t>
-  </si>
-  <si>
-    <t>1341</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>4214</t>
+    <t>35</t>
+  </si>
+  <si>
+    <t>73</t>
+  </si>
+  <si>
+    <t>222</t>
+  </si>
+  <si>
+    <t>1285</t>
   </si>
 </sst>
 </file>
@@ -443,15 +422,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="24.21875" style="2" customWidth="1"/>
     <col min="2" max="2" width="10.33203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="14.44140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="13.6640625" style="2" customWidth="1"/>
@@ -488,71 +467,28 @@
         <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{B3D7B355-646B-4033-98B0-02126804DE2F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>